<commit_message>
Job Hit Map sample
</commit_message>
<xml_diff>
--- a/output/Job HitMap Sample.xlsx
+++ b/output/Job HitMap Sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6431dddeb4959f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6431dddeb4959f/Documents/UiPath/Diamond/sct9-diamond-proj2/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{AE01B63A-DD5C-4383-BF54-D2B6D9100EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D12C376-9D0B-457B-B44D-7F164978E88D}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{AE01B63A-DD5C-4383-BF54-D2B6D9100EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED6BF249-DAEA-4DB0-BD0F-82DAEFDE4CE0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{E48EDA91-AB83-457D-86A2-28B860ABBB36}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1439,7 +1439,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1717,7 +1717,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>